<commit_message>
feat: Tugas kelompok, Accuracy, Precision, Recall, F1-Score
</commit_message>
<xml_diff>
--- a/hasil_perbandingan.xlsx
+++ b/hasil_perbandingan.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,25 +447,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>F1-Score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>AUC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>TP</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>TN</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>FP</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>FN</t>
         </is>
@@ -481,18 +496,27 @@
         <v>0.7252747252747253</v>
       </c>
       <c r="C2" t="n">
+        <v>0.7659574468085106</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7422680412371134</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.7258536585365853</v>
       </c>
-      <c r="D2" t="n">
+      <c r="G2" t="n">
         <v>36</v>
       </c>
-      <c r="E2" t="n">
+      <c r="H2" t="n">
         <v>30</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>11</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>14</v>
       </c>
     </row>
@@ -506,18 +530,27 @@
         <v>0.7912087912087912</v>
       </c>
       <c r="C3" t="n">
+        <v>0.7924528301886793</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8155339805825242</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.8680487804878049</v>
       </c>
-      <c r="D3" t="n">
+      <c r="G3" t="n">
         <v>42</v>
       </c>
-      <c r="E3" t="n">
+      <c r="H3" t="n">
         <v>30</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>11</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -531,18 +564,27 @@
         <v>0.7472527472527473</v>
       </c>
       <c r="C4" t="n">
+        <v>0.7547169811320755</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.7766990291262136</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.8595121951219512</v>
       </c>
-      <c r="D4" t="n">
+      <c r="G4" t="n">
         <v>40</v>
       </c>
-      <c r="E4" t="n">
+      <c r="H4" t="n">
         <v>28</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
         <v>13</v>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>